<commit_message>
functionality added to store data on db
</commit_message>
<xml_diff>
--- a/productionPlanning/I4_part_SPM_operations.xlsx
+++ b/productionPlanning/I4_part_SPM_operations.xlsx
@@ -20,7 +20,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="53">
+  <si>
+    <t xml:space="preserve">Material Code</t>
+  </si>
   <si>
     <t xml:space="preserve">Part No.</t>
   </si>
@@ -130,6 +133,9 @@
     <t xml:space="preserve">0.50/0.60</t>
   </si>
   <si>
+    <t xml:space="preserve">YJC-61121(NEW)</t>
+  </si>
+  <si>
     <t xml:space="preserve">YJC-61171</t>
   </si>
   <si>
@@ -160,10 +166,19 @@
     <t xml:space="preserve">YE3-K10-58311</t>
   </si>
   <si>
+    <t xml:space="preserve">YE3-K10-58311/411</t>
+  </si>
+  <si>
+    <t xml:space="preserve">YE3-K10-58411</t>
+  </si>
+  <si>
+    <t xml:space="preserve">YE3-58311</t>
+  </si>
+  <si>
     <t xml:space="preserve">YE3-58311/411</t>
   </si>
   <si>
-    <t xml:space="preserve">YE3-K10-58411</t>
+    <t xml:space="preserve">YE3-58411</t>
   </si>
 </sst>
 </file>
@@ -283,18 +298,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H20"/>
+  <dimension ref="A1:I35"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B18" activeCellId="0" sqref="B18"/>
+      <selection pane="topLeft" activeCell="B29" activeCellId="0" sqref="B29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="27.41"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="4" style="0" width="14.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="22.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="27.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="17.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="5" style="0" width="14.08"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -322,48 +337,54 @@
       <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
-        <v>8</v>
+      <c r="A2" s="2" t="n">
+        <v>2149061</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" s="2" t="n">
+        <v>9</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="D2" s="2" t="n">
-        <v>4</v>
-      </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="2" t="n">
+        <v>2085566</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="2" t="n">
         <v>9</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" s="2" t="n">
-        <v>9</v>
-      </c>
-      <c r="D3" s="2" t="n">
+      <c r="E3" s="2" t="n">
         <v>5</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>14</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>15</v>
@@ -374,22 +395,25 @@
       <c r="H3" s="2" t="s">
         <v>17</v>
       </c>
+      <c r="I3" s="2" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2" t="s">
-        <v>18</v>
+      <c r="A4" s="2" t="n">
+        <v>2085565</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4" s="2" t="n">
+        <v>19</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="2" t="n">
         <v>9</v>
       </c>
-      <c r="D4" s="2" t="n">
+      <c r="E4" s="2" t="n">
         <v>5</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>14</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>15</v>
@@ -400,22 +424,25 @@
       <c r="H4" s="2" t="s">
         <v>17</v>
       </c>
+      <c r="I4" s="2" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="2" t="s">
-        <v>19</v>
+      <c r="A5" s="2" t="n">
+        <v>2167770</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C5" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="2" t="n">
         <v>10.17</v>
       </c>
-      <c r="D5" s="2" t="n">
-        <v>4</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>9</v>
+      <c r="E5" s="2" t="n">
+        <v>4</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>10</v>
@@ -426,22 +453,25 @@
       <c r="H5" s="2" t="s">
         <v>12</v>
       </c>
+      <c r="I5" s="2" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="2" t="s">
-        <v>20</v>
+      <c r="A6" s="2" t="n">
+        <v>2051469</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C6" s="2" t="n">
+        <v>21</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" s="2" t="n">
         <v>8</v>
       </c>
-      <c r="D6" s="2" t="n">
-        <v>4</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>9</v>
+      <c r="E6" s="2" t="n">
+        <v>4</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>10</v>
@@ -452,22 +482,25 @@
       <c r="H6" s="2" t="s">
         <v>12</v>
       </c>
+      <c r="I6" s="2" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="2" t="s">
-        <v>21</v>
+      <c r="A7" s="2" t="n">
+        <v>2051470</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C7" s="2" t="n">
+        <v>22</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="2" t="n">
         <v>8</v>
       </c>
-      <c r="D7" s="2" t="n">
-        <v>4</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>9</v>
+      <c r="E7" s="2" t="n">
+        <v>4</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>10</v>
@@ -478,22 +511,25 @@
       <c r="H7" s="2" t="s">
         <v>12</v>
       </c>
+      <c r="I7" s="2" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="2" t="s">
-        <v>22</v>
+      <c r="A8" s="2" t="n">
+        <v>2122174</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C8" s="2" t="n">
+      <c r="C8" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" s="2" t="n">
         <v>8</v>
       </c>
-      <c r="D8" s="2" t="n">
-        <v>4</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>9</v>
+      <c r="E8" s="2" t="n">
+        <v>4</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>10</v>
@@ -504,22 +540,25 @@
       <c r="H8" s="2" t="s">
         <v>12</v>
       </c>
+      <c r="I8" s="2" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="2" t="n">
+        <v>2122175</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C9" s="2" t="n">
+      <c r="D9" s="2" t="n">
         <v>8</v>
       </c>
-      <c r="D9" s="2" t="n">
-        <v>4</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>9</v>
+      <c r="E9" s="2" t="n">
+        <v>4</v>
       </c>
       <c r="F9" s="2" t="s">
         <v>10</v>
@@ -530,22 +569,25 @@
       <c r="H9" s="2" t="s">
         <v>12</v>
       </c>
+      <c r="I9" s="2" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="2" t="s">
-        <v>25</v>
+      <c r="A10" s="2" t="n">
+        <v>2079693</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C10" s="2" t="n">
+      <c r="C10" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10" s="2" t="n">
         <v>6.5</v>
       </c>
-      <c r="D10" s="2" t="n">
-        <v>4</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>9</v>
+      <c r="E10" s="2" t="n">
+        <v>4</v>
       </c>
       <c r="F10" s="2" t="s">
         <v>10</v>
@@ -556,22 +598,25 @@
       <c r="H10" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="11" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="2" t="s">
+      <c r="I10" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="2" t="n">
+        <v>2079696</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C11" s="2" t="n">
+      <c r="D11" s="2" t="n">
         <v>6.5</v>
       </c>
-      <c r="D11" s="2" t="n">
-        <v>4</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>9</v>
+      <c r="E11" s="2" t="n">
+        <v>4</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>10</v>
@@ -582,74 +627,83 @@
       <c r="H11" s="2" t="s">
         <v>12</v>
       </c>
+      <c r="I11" s="2" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="2" t="s">
-        <v>28</v>
+      <c r="A12" s="2" t="n">
+        <v>2120460</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C12" s="2" t="n">
+      <c r="C12" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D12" s="2" t="n">
         <v>9</v>
       </c>
-      <c r="D12" s="2" t="n">
-        <v>4</v>
-      </c>
-      <c r="E12" s="2" t="s">
+      <c r="E12" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="2" t="n">
+        <v>2120464</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D13" s="2" t="n">
         <v>9</v>
       </c>
-      <c r="F12" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="H12" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C13" s="2" t="n">
+      <c r="E13" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="2" t="n">
+        <v>2134665</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D14" s="2" t="n">
         <v>9</v>
       </c>
-      <c r="D13" s="2" t="n">
-        <v>4</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="H13" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="C14" s="2" t="n">
-        <v>9</v>
-      </c>
-      <c r="D14" s="2" t="n">
+      <c r="E14" s="2" t="n">
         <v>5</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>32</v>
       </c>
       <c r="F14" s="2" t="s">
         <v>33</v>
@@ -660,22 +714,25 @@
       <c r="H14" s="2" t="s">
         <v>35</v>
       </c>
+      <c r="I14" s="2" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="2" t="s">
-        <v>36</v>
+      <c r="A15" s="2" t="n">
+        <v>2257584</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C15" s="2" t="n">
+        <v>37</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D15" s="2" t="n">
         <v>8.45</v>
       </c>
-      <c r="D15" s="2" t="n">
+      <c r="E15" s="2" t="n">
         <v>5</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>32</v>
       </c>
       <c r="F15" s="2" t="s">
         <v>33</v>
@@ -686,136 +743,289 @@
       <c r="H15" s="2" t="s">
         <v>35</v>
       </c>
+      <c r="I15" s="2" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="2" t="s">
-        <v>37</v>
+      <c r="A16" s="2" t="n">
+        <v>2134668</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C16" s="2" t="n">
+      <c r="C16" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D16" s="2" t="n">
+        <v>8.45</v>
+      </c>
+      <c r="E16" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="2" t="n">
+        <v>2118357</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D17" s="2" t="n">
         <v>10.53</v>
       </c>
-      <c r="D16" s="2" t="n">
-        <v>4</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G16" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="H16" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C17" s="2" t="n">
+      <c r="E17" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="2" t="n">
+        <v>2118358</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D18" s="2" t="n">
         <v>10.53</v>
       </c>
-      <c r="D17" s="2" t="n">
-        <v>4</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G17" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="H17" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C18" s="2" t="n">
+      <c r="E18" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="2" t="n">
+        <v>2068711</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D19" s="2" t="n">
         <v>8</v>
       </c>
-      <c r="D18" s="2" t="n">
+      <c r="E19" s="2" t="n">
         <v>3</v>
       </c>
-      <c r="E18" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="G18" s="2" t="s">
+      <c r="F19" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="H18" s="2" t="s">
+      <c r="G19" s="2" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="19" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="2" t="s">
+      <c r="H19" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="I19" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C19" s="2" t="n">
+    </row>
+    <row r="20" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="2" t="n">
+        <v>2066304</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D20" s="2" t="n">
         <v>8</v>
       </c>
-      <c r="D19" s="2" t="n">
-        <v>4</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G19" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="H19" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="C20" s="2" t="n">
+      <c r="E20" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I20" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="2" t="n">
+        <v>2066305</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D21" s="2" t="n">
         <v>8</v>
       </c>
-      <c r="D20" s="2" t="n">
-        <v>4</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G20" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="H20" s="2" t="s">
-        <v>12</v>
-      </c>
+      <c r="E21" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I21" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="2" t="n">
+        <v>2032029</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D22" s="2" t="n">
+        <v>8</v>
+      </c>
+      <c r="E22" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I22" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="2" t="n">
+        <v>2032033</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D23" s="2" t="n">
+        <v>8</v>
+      </c>
+      <c r="E23" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I23" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
+    </row>
+    <row r="25" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B25" s="2"/>
+      <c r="C25" s="2"/>
+    </row>
+    <row r="26" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B26" s="2"/>
+      <c r="C26" s="2"/>
+    </row>
+    <row r="27" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B27" s="2"/>
+      <c r="C27" s="2"/>
+    </row>
+    <row r="28" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B28" s="2"/>
+      <c r="C28" s="2"/>
+    </row>
+    <row r="29" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B29" s="2"/>
+      <c r="C29" s="2"/>
+    </row>
+    <row r="30" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B30" s="2"/>
+      <c r="C30" s="2"/>
+    </row>
+    <row r="31" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B31" s="2"/>
+      <c r="C31" s="2"/>
+    </row>
+    <row r="32" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B32" s="2"/>
+      <c r="C32" s="2"/>
+    </row>
+    <row r="33" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B33" s="2"/>
+      <c r="C33" s="2"/>
+    </row>
+    <row r="34" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B34" s="2"/>
+      <c r="C34" s="2"/>
+    </row>
+    <row r="35" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B35" s="2"/>
+      <c r="C35" s="2"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>